<commit_message>
Change in TestCase for SmokeSanity in SNCH SmokeSanityTestCases_SNCH.xlsx
</commit_message>
<xml_diff>
--- a/Library/SmokeSanityTestCases_SNCH.xlsx
+++ b/Library/SmokeSanityTestCases_SNCH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA\AutomationTest\Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\AutomationTest\Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Appointment\TC002CreateAppointmentFollowup.py</t>
   </si>
   <si>
-    <t>Reports\TC003SalesDayBookReport.py</t>
-  </si>
-  <si>
     <t>TC007</t>
   </si>
   <si>
@@ -88,15 +85,9 @@
     <t>TC009</t>
   </si>
   <si>
-    <t>Reports\TC006PatientCreditSummaryReport.py</t>
-  </si>
-  <si>
     <t>TC010</t>
   </si>
   <si>
-    <t>Reports\TC007DoctorSummaryReport.py</t>
-  </si>
-  <si>
     <t>TC011</t>
   </si>
   <si>
@@ -118,12 +109,6 @@
     <t>TC014</t>
   </si>
   <si>
-    <t>TC016</t>
-  </si>
-  <si>
-    <t>TC017</t>
-  </si>
-  <si>
     <t>Laboratory\TC005GenerateLabReport.py</t>
   </si>
   <si>
@@ -200,6 +185,9 @@
   </si>
   <si>
     <t>Billing\OPbilling\TC002OPDbillingLabXray.py</t>
+  </si>
+  <si>
+    <t>Reports\TC011UserCollectionReport.py</t>
   </si>
 </sst>
 </file>
@@ -575,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +589,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -610,10 +598,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -621,7 +609,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -635,7 +623,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -643,7 +631,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -652,20 +640,20 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -679,15 +667,15 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -701,15 +689,15 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -723,15 +711,15 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -745,7 +733,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -753,7 +741,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -762,20 +750,20 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
@@ -784,20 +772,20 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
@@ -806,12 +794,12 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -819,7 +807,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>6</v>
@@ -828,12 +816,12 @@
         <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -841,7 +829,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
@@ -850,42 +838,42 @@
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>13</v>
@@ -894,20 +882,20 @@
         <v>0</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
@@ -916,20 +904,20 @@
         <v>0</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>13</v>
@@ -938,20 +926,20 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>13</v>
@@ -960,56 +948,12 @@
         <v>0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1034,13 +978,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1048,7 +992,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -1057,7 +1001,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1066,7 +1010,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -1075,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -1084,7 +1028,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -1093,7 +1037,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -1102,7 +1046,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -1111,7 +1055,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -1120,7 +1064,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -1129,7 +1073,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -1138,7 +1082,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2"/>
     </row>

</xml_diff>